<commit_message>
Validación Importar Insumos Pt1
Validaciones: Que sean Números, que existan las id correspondientes. Tambien se añadio un titulo para los modulos y se agrego la pagina para ver parametros
</commit_message>
<xml_diff>
--- a/vistas/doc/plantillaInsumos.xlsx
+++ b/vistas/doc/plantillaInsumos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kardex\vistas\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0964E403-F25C-453D-8AEA-6F26215C6256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{694D2ED9-E1DD-4A87-AA9D-B8F6617E7B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{B4CA8B5D-F8B6-4673-B6FE-DE551AF2E515}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B4CA8B5D-F8B6-4673-B6FE-DE551AF2E515}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -40,75 +40,220 @@
     <author>Admin</author>
   </authors>
   <commentList>
-    <comment ref="L3" authorId="0" shapeId="0" xr:uid="{1DE9270E-C2D6-4A24-9F13-8B338321BA08}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Ejemplo, ingresa una caja de lapiz</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="M3" authorId="0" shapeId="0" xr:uid="{DCD2E247-6E8D-475B-A331-212F2684C955}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Ej: La caja de lapiz tiene 6 unidades</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N3" authorId="0" shapeId="0" xr:uid="{5CEE68A5-07B0-4526-A800-C5EE72252547}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Ej: Si una caja de lapiz tiene 6 unidades, el valor seria 6</t>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{1B0148A9-D2CC-4A97-B866-7005CB5BC432}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+stock para requisición o venta</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{31BE634C-F40A-4E4F-B9B4-8622E15217ED}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+stock que ingresa a bodega por facturas o importación</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{A61BA151-5E73-4246-B35F-353BAFE0A852}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+precio de adquisicion por proveedores en sus facturas</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{7E659C1F-B4DC-4E79-AA17-67F21A37714D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+precio para venta</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{BFF2DF60-0917-4C03-B60D-B1FBB7CADB51}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+precio especial para venta al por mayor</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{FF395F09-2779-4AC4-8869-AC1CA0C1001F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ej: ingresa una caja de lapices, esta tiene 6 unidades de lapices, el valor seria: Caja, buscar que id tiene este valor y colocar el numero</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{FB331A6B-F094-47B8-9AAE-DA8E8169BF21}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ej: ingresa una caja de lapices, esta tiene 6 unidades de lapices, el valor seria: Unidad, buscar que id tiene este valor y colocar el numero</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{48BE2CF4-40F9-4D4B-B03E-499B6AB3A81D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ej: una caja de lapices tiene 6 lapices, el valor seria: 6</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{60D9A62E-A9D8-4AED-97A3-7D68B264C630}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Admin:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1: para habilitar el insumo
+0: para que no aparezca en requisicion o venta</t>
         </r>
       </text>
     </comment>
@@ -119,55 +264,55 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
-    <t>ID_CATEGORIA</t>
-  </si>
-  <si>
-    <t>CODIGO</t>
-  </si>
-  <si>
-    <t>DESCRIPCION</t>
-  </si>
-  <si>
-    <t>OBSERVACION</t>
-  </si>
-  <si>
-    <t>STOCK</t>
-  </si>
-  <si>
-    <t>PRECIO_COMPRA</t>
-  </si>
-  <si>
-    <t>ESTANTE</t>
-  </si>
-  <si>
-    <t>NIVEL</t>
-  </si>
-  <si>
-    <t>SECCION</t>
-  </si>
-  <si>
-    <t>PRIORIDAD</t>
-  </si>
-  <si>
-    <t>UNIDAD_ENT</t>
-  </si>
-  <si>
-    <t>UNIDAD_SAL</t>
-  </si>
-  <si>
-    <t>CONTENIDO</t>
-  </si>
-  <si>
-    <t>EJ:</t>
-  </si>
-  <si>
-    <t>SA-1</t>
-  </si>
-  <si>
-    <t>LAPICERO NEGRO</t>
-  </si>
-  <si>
-    <t>PUNTA FINA</t>
+    <t>id_categoria(INT)</t>
+  </si>
+  <si>
+    <t>codigo(VARCHAR)</t>
+  </si>
+  <si>
+    <t>descripcion(TEXT)</t>
+  </si>
+  <si>
+    <t>observacion(TEXT)</t>
+  </si>
+  <si>
+    <t>stock(INT)</t>
+  </si>
+  <si>
+    <t>stockIn(INT)</t>
+  </si>
+  <si>
+    <t>precio_compra(FLOAT)</t>
+  </si>
+  <si>
+    <t>precio_unidad(FLOAT)</t>
+  </si>
+  <si>
+    <t>precio_por_mayor(FLOAT)</t>
+  </si>
+  <si>
+    <t>estante(CHAR)</t>
+  </si>
+  <si>
+    <t>nivel(CHAR)</t>
+  </si>
+  <si>
+    <t>seccion(CHAR)</t>
+  </si>
+  <si>
+    <t>prioridad(INT)</t>
+  </si>
+  <si>
+    <t>unidad(INT)</t>
+  </si>
+  <si>
+    <t>unidadSal(INT)</t>
+  </si>
+  <si>
+    <t>contenido(INT)</t>
+  </si>
+  <si>
+    <t>habilitado(INT)</t>
   </si>
 </sst>
 </file>
@@ -222,7 +367,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -532,111 +688,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F89F08D-C9D3-4F4B-9025-7CE6006A7692}">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
         <v>13</v>
       </c>
-      <c r="B1">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>500</v>
-      </c>
-      <c r="H1">
-        <v>6</v>
-      </c>
-      <c r="I1">
-        <v>2</v>
-      </c>
-      <c r="J1">
-        <v>1</v>
-      </c>
-      <c r="K1">
-        <v>1</v>
-      </c>
-      <c r="L1">
-        <v>1</v>
-      </c>
-      <c r="M1">
-        <v>6</v>
-      </c>
-      <c r="N1">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L3" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" t="s">
-        <v>11</v>
-      </c>
-      <c r="N3" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B2:B121">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
13. Modificado Año Actual
El valor de Año actual es almacenado en la variable Session por tanto se modifican todas las funciones donde aplique el tema de fecha, desde los archivos en los modulos, ajax, controladores. js
</commit_message>
<xml_diff>
--- a/vistas/doc/plantillaInsumos.xlsx
+++ b/vistas/doc/plantillaInsumos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\kardex\vistas\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{694D2ED9-E1DD-4A87-AA9D-B8F6617E7B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9D7DAF24-6D10-4459-86EF-BEEE08A79081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{B4CA8B5D-F8B6-4673-B6FE-DE551AF2E515}"/>
+    <workbookView xWindow="3270" yWindow="5205" windowWidth="18000" windowHeight="9480" xr2:uid="{B4CA8B5D-F8B6-4673-B6FE-DE551AF2E515}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -64,103 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{31BE634C-F40A-4E4F-B9B4-8622E15217ED}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-stock que ingresa a bodega por facturas o importación</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{A61BA151-5E73-4246-B35F-353BAFE0A852}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-precio de adquisicion por proveedores en sus facturas</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{7E659C1F-B4DC-4E79-AA17-67F21A37714D}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-precio para venta</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{BFF2DF60-0917-4C03-B60D-B1FBB7CADB51}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-precio especial para venta al por mayor</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{FF395F09-2779-4AC4-8869-AC1CA0C1001F}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{FF395F09-2779-4AC4-8869-AC1CA0C1001F}">
       <text>
         <r>
           <rPr>
@@ -184,31 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{FB331A6B-F094-47B8-9AAE-DA8E8169BF21}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-ej: ingresa una caja de lapices, esta tiene 6 unidades de lapices, el valor seria: Unidad, buscar que id tiene este valor y colocar el numero</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{48BE2CF4-40F9-4D4B-B03E-499B6AB3A81D}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{48BE2CF4-40F9-4D4B-B03E-499B6AB3A81D}">
       <text>
         <r>
           <rPr>
@@ -232,37 +112,12 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{60D9A62E-A9D8-4AED-97A3-7D68B264C630}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Admin:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-1: para habilitar el insumo
-0: para que no aparezca en requisicion o venta</t>
-        </r>
-      </text>
-    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>id_categoria(INT)</t>
   </si>
@@ -279,18 +134,6 @@
     <t>stock(INT)</t>
   </si>
   <si>
-    <t>stockIn(INT)</t>
-  </si>
-  <si>
-    <t>precio_compra(FLOAT)</t>
-  </si>
-  <si>
-    <t>precio_unidad(FLOAT)</t>
-  </si>
-  <si>
-    <t>precio_por_mayor(FLOAT)</t>
-  </si>
-  <si>
     <t>estante(CHAR)</t>
   </si>
   <si>
@@ -300,19 +143,10 @@
     <t>seccion(CHAR)</t>
   </si>
   <si>
-    <t>prioridad(INT)</t>
-  </si>
-  <si>
     <t>unidad(INT)</t>
   </si>
   <si>
-    <t>unidadSal(INT)</t>
-  </si>
-  <si>
     <t>contenido(INT)</t>
-  </si>
-  <si>
-    <t>habilitado(INT)</t>
   </si>
 </sst>
 </file>
@@ -688,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F89F08D-C9D3-4F4B-9025-7CE6006A7692}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,19 +534,13 @@
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -743,31 +571,10 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B121">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  <conditionalFormatting sqref="B2:B120">
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>